<commit_message>
[feat] UI 추가 및 ItemObject Prefab 추가
</commit_message>
<xml_diff>
--- a/SpartaFarming/Util/excel_files/ItemInfo.xlsx
+++ b/SpartaFarming/Util/excel_files/ItemInfo.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sudo\Documents\GitHub\SpartaFarming\SpartaFarming\Util\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E969F0A-75E3-4B28-BE2E-531E24DA148F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F2C264-60F6-4931-BFE2-687824076AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4755" yWindow="4635" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -236,23 +236,47 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>당근</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>Seed</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>CarrotSeed</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprite/Seed/CarrotSeed</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefab/Seed/CarrotSeed</t>
+    <t>Beet</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>비트</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Seed/BeetSeed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Seed/BeetSeed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wheat</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>밀</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Seed/WheatSeed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Seed/WheatSeed</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>price</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Price</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -831,10 +855,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -852,7 +876,7 @@
     <col min="12" max="12" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -889,8 +913,11 @@
       <c r="L1" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" customHeight="1">
+      <c r="M1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -927,8 +954,11 @@
       <c r="L2" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -965,25 +995,28 @@
       <c r="L3" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="E4" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G4">
         <v>-1</v>
@@ -1001,150 +1034,162 @@
         <v>0</v>
       </c>
       <c r="L4">
+        <v>999</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>999</v>
+      </c>
+      <c r="M5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="5">
+        <v>-1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>999</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>30</v>
+      </c>
+      <c r="L7">
+        <v>999</v>
+      </c>
+      <c r="M7">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="5">
-        <v>-1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1">
-        <v>2000</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6">
-        <v>-1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>20</v>
-      </c>
-      <c r="K6">
+    <row r="8" spans="1:13">
+      <c r="A8" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1">
-        <v>3000</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="G7">
-        <v>64</v>
-      </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1">
-        <v>4000</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="G8">
         <v>64</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1155,34 +1200,37 @@
       <c r="L8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9">
-        <v>-1</v>
+        <v>64</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1193,40 +1241,77 @@
       <c r="L9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="B12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="B15"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="B16"/>
       <c r="D16" s="5"/>
     </row>

</xml_diff>

<commit_message>
[feat] changed player with system
</commit_message>
<xml_diff>
--- a/SpartaFarming/Util/excel_files/ItemInfo.xlsx
+++ b/SpartaFarming/Util/excel_files/ItemInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sparta\SpartaFarming\SpartaFarming\Util\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anbak\SpartaFarming\SpartaFarming\Util\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791341B6-1B41-4E71-B248-63BBB9C9B02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A681357-8774-4179-BF34-BFE21CAF0741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10035" yWindow="3960" windowWidth="21825" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15585" yWindow="4545" windowWidth="19470" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>ID</t>
   </si>
@@ -325,6 +325,102 @@
   </si>
   <si>
     <t>Prefab/Resource/Gold</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hoe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Axe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PickAxe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>FishingRod</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>WateringCan</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fence</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>물뿌리개</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>울타리</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚시대</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>곡괭이</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>도끼</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>낫</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Tool/Hoe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Tool/Hoe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Tool/Axe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Tool/PickAxe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Tool/FishingRod</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Tool/Fence</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/Tool/WateringCan</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Tool/WateringCan</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Tool/Fence</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Tool/FishingRod</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Tool/PickAxe</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefab/Tool/Axe</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -903,10 +999,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -1377,31 +1473,31 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1">
-        <v>4000</v>
+        <v>3001</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>89</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="G12">
         <v>64</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1418,28 +1514,28 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1">
-        <v>5000</v>
+        <v>3002</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>35</v>
+        <v>88</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="G13">
-        <v>-1</v>
+        <v>64</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1454,45 +1550,291 @@
         <v>1</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="B15" s="5"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18"/>
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20"/>
+      <c r="A14" s="1">
+        <v>3003</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>64</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18" customHeight="1">
+      <c r="A15" s="1">
+        <v>3004</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G15">
+        <v>64</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" customHeight="1">
+      <c r="A16" s="1">
+        <v>3005</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16">
+        <v>64</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1">
+      <c r="A17" s="1">
+        <v>3006</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17">
+        <v>64</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18">
+        <v>64</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="5"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="B21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="B24"/>
+      <c r="C24"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="B25"/>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="B26"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E20">
-    <sortCondition ref="A4:A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:E26">
+    <sortCondition ref="A4:A26"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>